<commit_message>
added Kastner atlas and scanner logs
</commit_message>
<xml_diff>
--- a/Logs/P03_scan_log.xlsx
+++ b/Logs/P03_scan_log.xlsx
@@ -41,9 +41,6 @@
     <t>loc</t>
   </si>
   <si>
-    <t xml:space="preserve">Participant Run </t>
-  </si>
-  <si>
     <t>Order Number</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>pa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mat file run number </t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,13 +396,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -410,7 +410,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>